<commit_message>
Da sua test case banr final
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\20181\Quan_tri_du_an\OneDrive_1_10-29-2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\20181\Quan_tri_du_an\Ngoc\Nha-thong-minh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DAFDDE4A-A1C2-496A-ABF1-58B1D6A1DE36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{018E2C8D-A42B-4689-8325-03100444CD7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="116">
   <si>
     <t>Online ID</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>BUG234</t>
+  </si>
+  <si>
+    <t>Ok da hoan thanh</t>
+  </si>
+  <si>
+    <t>chua hoan thanh, can lam lai</t>
   </si>
 </sst>
 </file>
@@ -1381,6 +1387,123 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1390,57 +1513,6 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1476,72 +1548,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3093,8 +3099,8 @@
   </sheetPr>
   <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3228,39 +3234,39 @@
       <c r="A7" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="178" t="s">
+      <c r="B7" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
+      <c r="C7" s="171"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="171"/>
+      <c r="J7" s="171"/>
+      <c r="K7" s="171"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1">
       <c r="A8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="138"/>
-      <c r="D8" s="137" t="s">
+      <c r="C8" s="135"/>
+      <c r="D8" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="138"/>
-      <c r="F8" s="137" t="s">
+      <c r="E8" s="135"/>
+      <c r="F8" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="138"/>
-      <c r="H8" s="179" t="s">
+      <c r="G8" s="135"/>
+      <c r="H8" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="179"/>
+      <c r="I8" s="158"/>
       <c r="J8" s="48" t="s">
         <v>30</v>
       </c>
@@ -3272,35 +3278,37 @@
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="166" t="s">
+      <c r="B9" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="167"/>
-      <c r="D9" s="172" t="s">
+      <c r="C9" s="138"/>
+      <c r="D9" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="173"/>
-      <c r="F9" s="154" t="s">
+      <c r="E9" s="162"/>
+      <c r="F9" s="176" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="155"/>
-      <c r="H9" s="183" t="s">
+      <c r="G9" s="177"/>
+      <c r="H9" s="159" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="184"/>
+      <c r="I9" s="160"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="134"/>
+      <c r="K9" s="173" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="168"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="175"/>
-      <c r="F10" s="156"/>
-      <c r="G10" s="157"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="164"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="179"/>
       <c r="H10" s="47" t="s">
         <v>34</v>
       </c>
@@ -3310,35 +3318,35 @@
       <c r="J10" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="135"/>
+      <c r="K10" s="174"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="168"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="174"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="157"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="179"/>
       <c r="H11" s="52" t="s">
         <v>70</v>
       </c>
       <c r="I11" s="52"/>
       <c r="J11" s="50"/>
-      <c r="K11" s="135"/>
+      <c r="K11" s="174"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="168"/>
-      <c r="C12" s="169"/>
-      <c r="D12" s="174"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="156"/>
-      <c r="G12" s="157"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="179"/>
       <c r="H12" s="47" t="s">
         <v>37</v>
       </c>
@@ -3346,45 +3354,45 @@
         <v>33</v>
       </c>
       <c r="J12" s="47"/>
-      <c r="K12" s="135"/>
+      <c r="K12" s="174"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="53">
         <v>981</v>
       </c>
-      <c r="B13" s="170"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="177"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="159"/>
+      <c r="B13" s="141"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="181"/>
       <c r="H13" s="55" t="s">
         <v>73</v>
       </c>
       <c r="I13" s="55"/>
       <c r="J13" s="56"/>
-      <c r="K13" s="136"/>
+      <c r="K13" s="175"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1">
       <c r="A14" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="137" t="s">
+      <c r="C14" s="135"/>
+      <c r="D14" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="138"/>
-      <c r="F14" s="137" t="s">
+      <c r="E14" s="135"/>
+      <c r="F14" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="138"/>
-      <c r="H14" s="179" t="s">
+      <c r="G14" s="135"/>
+      <c r="H14" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="179"/>
+      <c r="I14" s="158"/>
       <c r="J14" s="122" t="s">
         <v>30</v>
       </c>
@@ -3396,37 +3404,39 @@
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="166" t="s">
+      <c r="B15" s="137" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="167"/>
-      <c r="D15" s="172" t="s">
+      <c r="C15" s="138"/>
+      <c r="D15" s="161" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="154" t="s">
+      <c r="E15" s="162"/>
+      <c r="F15" s="176" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="155"/>
-      <c r="H15" s="183" t="s">
+      <c r="G15" s="177"/>
+      <c r="H15" s="159" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="184"/>
+      <c r="I15" s="160"/>
       <c r="J15" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="134"/>
+      <c r="K15" s="173" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="168"/>
-      <c r="C16" s="169"/>
-      <c r="D16" s="174"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="157"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="179"/>
       <c r="H16" s="121" t="s">
         <v>34</v>
       </c>
@@ -3436,18 +3446,18 @@
       <c r="J16" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="135"/>
+      <c r="K16" s="174"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="168"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="174"/>
-      <c r="E17" s="175"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="157"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="140"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="164"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="179"/>
       <c r="H17" s="52" t="s">
         <v>70</v>
       </c>
@@ -3457,18 +3467,18 @@
       <c r="J17" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="135"/>
+      <c r="K17" s="174"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="168"/>
-      <c r="C18" s="169"/>
-      <c r="D18" s="174"/>
-      <c r="E18" s="175"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="157"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="140"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="178"/>
+      <c r="G18" s="179"/>
       <c r="H18" s="121" t="s">
         <v>37</v>
       </c>
@@ -3476,18 +3486,18 @@
         <v>33</v>
       </c>
       <c r="J18" s="121"/>
-      <c r="K18" s="135"/>
+      <c r="K18" s="174"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="53">
         <v>982</v>
       </c>
-      <c r="B19" s="170"/>
-      <c r="C19" s="171"/>
-      <c r="D19" s="176"/>
-      <c r="E19" s="177"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="159"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="166"/>
+      <c r="F19" s="180"/>
+      <c r="G19" s="181"/>
       <c r="H19" s="55" t="s">
         <v>73</v>
       </c>
@@ -3495,28 +3505,28 @@
         <v>73</v>
       </c>
       <c r="J19" s="56"/>
-      <c r="K19" s="136"/>
+      <c r="K19" s="175"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="181" t="s">
+      <c r="B20" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="182"/>
-      <c r="D20" s="181" t="s">
+      <c r="C20" s="145"/>
+      <c r="D20" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="182"/>
-      <c r="F20" s="181" t="s">
+      <c r="E20" s="145"/>
+      <c r="F20" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="182"/>
-      <c r="H20" s="187" t="s">
+      <c r="G20" s="145"/>
+      <c r="H20" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="187"/>
+      <c r="I20" s="143"/>
       <c r="J20" s="59" t="s">
         <v>30</v>
       </c>
@@ -3528,37 +3538,37 @@
       <c r="A21" s="50">
         <v>3</v>
       </c>
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="146" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="146" t="s">
+      <c r="C21" s="147"/>
+      <c r="D21" s="152" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="147"/>
-      <c r="F21" s="160" t="s">
+      <c r="E21" s="153"/>
+      <c r="F21" s="182" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="161"/>
-      <c r="H21" s="152" t="s">
+      <c r="G21" s="183"/>
+      <c r="H21" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="153"/>
+      <c r="I21" s="168"/>
       <c r="J21" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="134"/>
+      <c r="K21" s="173"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="142"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="149"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="163"/>
+      <c r="B22" s="148"/>
+      <c r="C22" s="149"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="155"/>
+      <c r="F22" s="184"/>
+      <c r="G22" s="185"/>
       <c r="H22" s="59" t="s">
         <v>34</v>
       </c>
@@ -3568,18 +3578,18 @@
       <c r="J22" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="135"/>
+      <c r="K22" s="174"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="142"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="162"/>
-      <c r="G23" s="163"/>
+      <c r="B23" s="148"/>
+      <c r="C23" s="149"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="184"/>
+      <c r="G23" s="185"/>
       <c r="H23" s="52" t="s">
         <v>71</v>
       </c>
@@ -3589,18 +3599,18 @@
       <c r="J23" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="135"/>
+      <c r="K23" s="174"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="142"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="149"/>
-      <c r="F24" s="162"/>
-      <c r="G24" s="163"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="149"/>
+      <c r="D24" s="154"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="184"/>
+      <c r="G24" s="185"/>
       <c r="H24" s="59" t="s">
         <v>37</v>
       </c>
@@ -3608,18 +3618,18 @@
         <v>33</v>
       </c>
       <c r="J24" s="59"/>
-      <c r="K24" s="135"/>
+      <c r="K24" s="174"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53">
         <v>921</v>
       </c>
-      <c r="B25" s="144"/>
-      <c r="C25" s="145"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="164"/>
-      <c r="G25" s="165"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="151"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
       <c r="H25" s="52" t="s">
         <v>73</v>
       </c>
@@ -3627,62 +3637,62 @@
         <v>74</v>
       </c>
       <c r="J25" s="50"/>
-      <c r="K25" s="135"/>
+      <c r="K25" s="174"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="180" t="s">
+      <c r="B26" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="180"/>
-      <c r="D26" s="178"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="178"/>
-      <c r="H26" s="178"/>
-      <c r="I26" s="178"/>
-      <c r="J26" s="178"/>
-      <c r="K26" s="178"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="171"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="171"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
+      <c r="K26" s="171"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="185" t="s">
+      <c r="B27" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="185"/>
-      <c r="D27" s="186"/>
-      <c r="E27" s="186"/>
-      <c r="F27" s="186"/>
-      <c r="G27" s="186"/>
-      <c r="H27" s="186"/>
-      <c r="I27" s="186"/>
-      <c r="J27" s="186"/>
-      <c r="K27" s="186"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="170"/>
+      <c r="E27" s="170"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="170"/>
+      <c r="I27" s="170"/>
+      <c r="J27" s="170"/>
+      <c r="K27" s="170"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="181" t="s">
+      <c r="B28" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="182"/>
-      <c r="D28" s="181" t="s">
+      <c r="C28" s="145"/>
+      <c r="D28" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="182"/>
-      <c r="F28" s="181" t="s">
+      <c r="E28" s="145"/>
+      <c r="F28" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="182"/>
-      <c r="H28" s="187" t="s">
+      <c r="G28" s="145"/>
+      <c r="H28" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="187"/>
+      <c r="I28" s="143"/>
       <c r="J28" s="59" t="s">
         <v>30</v>
       </c>
@@ -3694,37 +3704,37 @@
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="140" t="s">
+      <c r="B29" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="141"/>
-      <c r="D29" s="146" t="s">
+      <c r="C29" s="147"/>
+      <c r="D29" s="152" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="147"/>
-      <c r="F29" s="146" t="s">
+      <c r="E29" s="153"/>
+      <c r="F29" s="152" t="s">
         <v>90</v>
       </c>
-      <c r="G29" s="147"/>
-      <c r="H29" s="183" t="s">
+      <c r="G29" s="153"/>
+      <c r="H29" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="184"/>
+      <c r="I29" s="160"/>
       <c r="J29" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="K29" s="134"/>
+      <c r="K29" s="173"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="142"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="148"/>
-      <c r="G30" s="149"/>
+      <c r="B30" s="148"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="154"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="59" t="s">
         <v>34</v>
       </c>
@@ -3734,18 +3744,18 @@
       <c r="J30" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="135"/>
+      <c r="K30" s="174"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="142"/>
-      <c r="C31" s="143"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="149"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="149"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="155"/>
       <c r="H31" s="52" t="s">
         <v>41</v>
       </c>
@@ -3755,18 +3765,18 @@
       <c r="J31" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K31" s="135"/>
+      <c r="K31" s="174"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="142"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="148"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="148"/>
-      <c r="G32" s="149"/>
+      <c r="B32" s="148"/>
+      <c r="C32" s="149"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="155"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="155"/>
       <c r="H32" s="59" t="s">
         <v>37</v>
       </c>
@@ -3774,18 +3784,18 @@
         <v>33</v>
       </c>
       <c r="J32" s="59"/>
-      <c r="K32" s="135"/>
+      <c r="K32" s="174"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="53">
         <v>922</v>
       </c>
-      <c r="B33" s="144"/>
-      <c r="C33" s="145"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="151"/>
-      <c r="F33" s="150"/>
-      <c r="G33" s="151"/>
+      <c r="B33" s="150"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="156"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="157"/>
       <c r="H33" s="52" t="s">
         <v>73</v>
       </c>
@@ -3793,28 +3803,28 @@
         <v>92</v>
       </c>
       <c r="J33" s="50"/>
-      <c r="K33" s="136"/>
+      <c r="K33" s="175"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="137" t="s">
+      <c r="B34" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="138"/>
-      <c r="D34" s="137" t="s">
+      <c r="C34" s="135"/>
+      <c r="D34" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="137" t="s">
+      <c r="E34" s="135"/>
+      <c r="F34" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="138"/>
-      <c r="H34" s="139" t="s">
+      <c r="G34" s="135"/>
+      <c r="H34" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="139"/>
+      <c r="I34" s="136"/>
       <c r="J34" s="47" t="s">
         <v>30</v>
       </c>
@@ -3826,37 +3836,37 @@
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="140" t="s">
+      <c r="B35" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="141"/>
-      <c r="D35" s="146" t="s">
+      <c r="C35" s="147"/>
+      <c r="D35" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="147"/>
-      <c r="F35" s="146" t="s">
+      <c r="E35" s="153"/>
+      <c r="F35" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="G35" s="147"/>
-      <c r="H35" s="152" t="s">
+      <c r="G35" s="153"/>
+      <c r="H35" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="I35" s="153"/>
+      <c r="I35" s="168"/>
       <c r="J35" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="K35" s="134"/>
+      <c r="K35" s="173"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="142"/>
-      <c r="C36" s="143"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="149"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="149"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="149"/>
+      <c r="D36" s="154"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="154"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="47" t="s">
         <v>34</v>
       </c>
@@ -3866,18 +3876,18 @@
       <c r="J36" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="K36" s="135"/>
+      <c r="K36" s="174"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="142"/>
-      <c r="C37" s="143"/>
-      <c r="D37" s="148"/>
-      <c r="E37" s="149"/>
-      <c r="F37" s="148"/>
-      <c r="G37" s="149"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="149"/>
+      <c r="D37" s="154"/>
+      <c r="E37" s="155"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="155"/>
       <c r="H37" s="52" t="s">
         <v>41</v>
       </c>
@@ -3887,18 +3897,18 @@
       <c r="J37" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K37" s="135"/>
+      <c r="K37" s="174"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="142"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="149"/>
-      <c r="F38" s="148"/>
-      <c r="G38" s="149"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="149"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="155"/>
+      <c r="F38" s="154"/>
+      <c r="G38" s="155"/>
       <c r="H38" s="47" t="s">
         <v>37</v>
       </c>
@@ -3906,18 +3916,18 @@
         <v>33</v>
       </c>
       <c r="J38" s="47"/>
-      <c r="K38" s="135"/>
+      <c r="K38" s="174"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="53">
         <v>823</v>
       </c>
-      <c r="B39" s="144"/>
-      <c r="C39" s="145"/>
-      <c r="D39" s="150"/>
-      <c r="E39" s="151"/>
-      <c r="F39" s="150"/>
-      <c r="G39" s="151"/>
+      <c r="B39" s="150"/>
+      <c r="C39" s="151"/>
+      <c r="D39" s="156"/>
+      <c r="E39" s="157"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="157"/>
       <c r="H39" s="52" t="s">
         <v>73</v>
       </c>
@@ -3925,7 +3935,7 @@
         <v>74</v>
       </c>
       <c r="J39" s="50"/>
-      <c r="K39" s="136"/>
+      <c r="K39" s="175"/>
     </row>
     <row r="40" spans="1:11" ht="10.5" customHeight="1">
       <c r="A40" s="53"/>
@@ -3944,22 +3954,22 @@
       <c r="A41" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="138"/>
-      <c r="D41" s="137" t="s">
+      <c r="C41" s="135"/>
+      <c r="D41" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="138"/>
-      <c r="F41" s="137" t="s">
+      <c r="E41" s="135"/>
+      <c r="F41" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="138"/>
-      <c r="H41" s="139" t="s">
+      <c r="G41" s="135"/>
+      <c r="H41" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I41" s="139"/>
+      <c r="I41" s="136"/>
       <c r="J41" s="47" t="s">
         <v>30</v>
       </c>
@@ -3971,35 +3981,35 @@
       <c r="A42" s="50">
         <v>6</v>
       </c>
-      <c r="B42" s="140" t="s">
+      <c r="B42" s="146" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="141"/>
-      <c r="D42" s="146" t="s">
+      <c r="C42" s="147"/>
+      <c r="D42" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="147"/>
-      <c r="F42" s="146" t="s">
+      <c r="E42" s="153"/>
+      <c r="F42" s="152" t="s">
         <v>99</v>
       </c>
-      <c r="G42" s="147"/>
-      <c r="H42" s="152" t="s">
+      <c r="G42" s="153"/>
+      <c r="H42" s="167" t="s">
         <v>100</v>
       </c>
-      <c r="I42" s="153"/>
+      <c r="I42" s="168"/>
       <c r="J42" s="54"/>
-      <c r="K42" s="134"/>
+      <c r="K42" s="173"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="142"/>
-      <c r="C43" s="143"/>
-      <c r="D43" s="148"/>
-      <c r="E43" s="149"/>
-      <c r="F43" s="148"/>
-      <c r="G43" s="149"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="149"/>
+      <c r="D43" s="154"/>
+      <c r="E43" s="155"/>
+      <c r="F43" s="154"/>
+      <c r="G43" s="155"/>
       <c r="H43" s="47" t="s">
         <v>34</v>
       </c>
@@ -4009,35 +4019,35 @@
       <c r="J43" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="K43" s="135"/>
+      <c r="K43" s="174"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="142"/>
-      <c r="C44" s="143"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="148"/>
-      <c r="G44" s="149"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="149"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="155"/>
+      <c r="F44" s="154"/>
+      <c r="G44" s="155"/>
       <c r="H44" s="52" t="s">
         <v>41</v>
       </c>
       <c r="I44" s="52"/>
       <c r="J44" s="50"/>
-      <c r="K44" s="135"/>
+      <c r="K44" s="174"/>
     </row>
     <row r="45" spans="1:11" ht="10.5" customHeight="1">
       <c r="A45" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="142"/>
-      <c r="C45" s="143"/>
-      <c r="D45" s="148"/>
-      <c r="E45" s="149"/>
-      <c r="F45" s="148"/>
-      <c r="G45" s="149"/>
+      <c r="B45" s="148"/>
+      <c r="C45" s="149"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="155"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="155"/>
       <c r="H45" s="47" t="s">
         <v>37</v>
       </c>
@@ -4045,45 +4055,45 @@
         <v>33</v>
       </c>
       <c r="J45" s="47"/>
-      <c r="K45" s="135"/>
+      <c r="K45" s="174"/>
     </row>
     <row r="46" spans="1:11" ht="10.5" customHeight="1">
       <c r="A46" s="53">
         <v>830</v>
       </c>
-      <c r="B46" s="144"/>
-      <c r="C46" s="145"/>
-      <c r="D46" s="150"/>
-      <c r="E46" s="151"/>
-      <c r="F46" s="150"/>
-      <c r="G46" s="151"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="151"/>
+      <c r="D46" s="156"/>
+      <c r="E46" s="157"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="157"/>
       <c r="H46" s="52" t="s">
         <v>40</v>
       </c>
       <c r="I46" s="52"/>
       <c r="J46" s="50"/>
-      <c r="K46" s="136"/>
+      <c r="K46" s="175"/>
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A47" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="138"/>
-      <c r="D47" s="137" t="s">
+      <c r="C47" s="135"/>
+      <c r="D47" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E47" s="138"/>
-      <c r="F47" s="137" t="s">
+      <c r="E47" s="135"/>
+      <c r="F47" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G47" s="138"/>
-      <c r="H47" s="139" t="s">
+      <c r="G47" s="135"/>
+      <c r="H47" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I47" s="139"/>
+      <c r="I47" s="136"/>
       <c r="J47" s="121" t="s">
         <v>30</v>
       </c>
@@ -4095,35 +4105,35 @@
       <c r="A48" s="50">
         <v>7</v>
       </c>
-      <c r="B48" s="140" t="s">
+      <c r="B48" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="141"/>
-      <c r="D48" s="146" t="s">
+      <c r="C48" s="147"/>
+      <c r="D48" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="E48" s="147"/>
-      <c r="F48" s="146" t="s">
+      <c r="E48" s="153"/>
+      <c r="F48" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="G48" s="147"/>
-      <c r="H48" s="152" t="s">
+      <c r="G48" s="153"/>
+      <c r="H48" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="I48" s="153"/>
+      <c r="I48" s="168"/>
       <c r="J48" s="54"/>
-      <c r="K48" s="134"/>
+      <c r="K48" s="173"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="142"/>
-      <c r="C49" s="143"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="149"/>
-      <c r="F49" s="148"/>
-      <c r="G49" s="149"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="149"/>
+      <c r="D49" s="154"/>
+      <c r="E49" s="155"/>
+      <c r="F49" s="154"/>
+      <c r="G49" s="155"/>
       <c r="H49" s="121" t="s">
         <v>34</v>
       </c>
@@ -4133,35 +4143,35 @@
       <c r="J49" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K49" s="135"/>
+      <c r="K49" s="174"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="142"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149"/>
-      <c r="F50" s="148"/>
-      <c r="G50" s="149"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="149"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="155"/>
+      <c r="F50" s="154"/>
+      <c r="G50" s="155"/>
       <c r="H50" s="52" t="s">
         <v>41</v>
       </c>
       <c r="I50" s="52"/>
       <c r="J50" s="50"/>
-      <c r="K50" s="135"/>
+      <c r="K50" s="174"/>
     </row>
     <row r="51" spans="1:11" ht="10.5" customHeight="1">
       <c r="A51" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="142"/>
-      <c r="C51" s="143"/>
-      <c r="D51" s="148"/>
-      <c r="E51" s="149"/>
-      <c r="F51" s="148"/>
-      <c r="G51" s="149"/>
+      <c r="B51" s="148"/>
+      <c r="C51" s="149"/>
+      <c r="D51" s="154"/>
+      <c r="E51" s="155"/>
+      <c r="F51" s="154"/>
+      <c r="G51" s="155"/>
       <c r="H51" s="121" t="s">
         <v>37</v>
       </c>
@@ -4169,45 +4179,45 @@
         <v>33</v>
       </c>
       <c r="J51" s="121"/>
-      <c r="K51" s="135"/>
+      <c r="K51" s="174"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1">
       <c r="A52" s="53">
         <v>827</v>
       </c>
-      <c r="B52" s="144"/>
-      <c r="C52" s="145"/>
-      <c r="D52" s="150"/>
-      <c r="E52" s="151"/>
-      <c r="F52" s="150"/>
-      <c r="G52" s="151"/>
+      <c r="B52" s="150"/>
+      <c r="C52" s="151"/>
+      <c r="D52" s="156"/>
+      <c r="E52" s="157"/>
+      <c r="F52" s="156"/>
+      <c r="G52" s="157"/>
       <c r="H52" s="52" t="s">
         <v>73</v>
       </c>
       <c r="I52" s="52"/>
       <c r="J52" s="50"/>
-      <c r="K52" s="136"/>
+      <c r="K52" s="175"/>
     </row>
     <row r="53" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A53" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B53" s="137" t="s">
+      <c r="B53" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="138"/>
-      <c r="D53" s="137" t="s">
+      <c r="C53" s="135"/>
+      <c r="D53" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E53" s="138"/>
-      <c r="F53" s="137" t="s">
+      <c r="E53" s="135"/>
+      <c r="F53" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G53" s="138"/>
-      <c r="H53" s="139" t="s">
+      <c r="G53" s="135"/>
+      <c r="H53" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I53" s="139"/>
+      <c r="I53" s="136"/>
       <c r="J53" s="121" t="s">
         <v>30</v>
       </c>
@@ -4219,37 +4229,37 @@
       <c r="A54" s="50">
         <v>8</v>
       </c>
-      <c r="B54" s="140" t="s">
+      <c r="B54" s="146" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="141"/>
-      <c r="D54" s="146" t="s">
+      <c r="C54" s="147"/>
+      <c r="D54" s="152" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="147"/>
-      <c r="F54" s="146" t="s">
+      <c r="E54" s="153"/>
+      <c r="F54" s="152" t="s">
         <v>106</v>
       </c>
-      <c r="G54" s="147"/>
-      <c r="H54" s="152" t="s">
+      <c r="G54" s="153"/>
+      <c r="H54" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="I54" s="153"/>
+      <c r="I54" s="168"/>
       <c r="J54" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="K54" s="134"/>
+      <c r="K54" s="173"/>
     </row>
     <row r="55" spans="1:11" ht="10.5" customHeight="1">
       <c r="A55" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="142"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="149"/>
-      <c r="F55" s="148"/>
-      <c r="G55" s="149"/>
+      <c r="B55" s="148"/>
+      <c r="C55" s="149"/>
+      <c r="D55" s="154"/>
+      <c r="E55" s="155"/>
+      <c r="F55" s="154"/>
+      <c r="G55" s="155"/>
       <c r="H55" s="121" t="s">
         <v>34</v>
       </c>
@@ -4259,18 +4269,18 @@
       <c r="J55" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K55" s="135"/>
+      <c r="K55" s="174"/>
     </row>
     <row r="56" spans="1:11" ht="10.5" customHeight="1">
       <c r="A56" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="142"/>
-      <c r="C56" s="143"/>
-      <c r="D56" s="148"/>
-      <c r="E56" s="149"/>
-      <c r="F56" s="148"/>
-      <c r="G56" s="149"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="149"/>
+      <c r="D56" s="154"/>
+      <c r="E56" s="155"/>
+      <c r="F56" s="154"/>
+      <c r="G56" s="155"/>
       <c r="H56" s="52" t="s">
         <v>70</v>
       </c>
@@ -4280,18 +4290,18 @@
       <c r="J56" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="K56" s="135"/>
+      <c r="K56" s="174"/>
     </row>
     <row r="57" spans="1:11" ht="10.5" customHeight="1">
       <c r="A57" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="142"/>
-      <c r="C57" s="143"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="149"/>
-      <c r="F57" s="148"/>
-      <c r="G57" s="149"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="149"/>
+      <c r="D57" s="154"/>
+      <c r="E57" s="155"/>
+      <c r="F57" s="154"/>
+      <c r="G57" s="155"/>
       <c r="H57" s="121" t="s">
         <v>37</v>
       </c>
@@ -4299,18 +4309,18 @@
         <v>33</v>
       </c>
       <c r="J57" s="121"/>
-      <c r="K57" s="135"/>
+      <c r="K57" s="174"/>
     </row>
     <row r="58" spans="1:11" ht="10.5" customHeight="1">
       <c r="A58" s="53">
         <v>829</v>
       </c>
-      <c r="B58" s="144"/>
-      <c r="C58" s="145"/>
-      <c r="D58" s="150"/>
-      <c r="E58" s="151"/>
-      <c r="F58" s="150"/>
-      <c r="G58" s="151"/>
+      <c r="B58" s="150"/>
+      <c r="C58" s="151"/>
+      <c r="D58" s="156"/>
+      <c r="E58" s="157"/>
+      <c r="F58" s="156"/>
+      <c r="G58" s="157"/>
       <c r="H58" s="52" t="s">
         <v>73</v>
       </c>
@@ -4318,28 +4328,28 @@
         <v>74</v>
       </c>
       <c r="J58" s="50"/>
-      <c r="K58" s="136"/>
+      <c r="K58" s="175"/>
     </row>
     <row r="59" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A59" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B59" s="137" t="s">
+      <c r="B59" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="138"/>
-      <c r="D59" s="137" t="s">
+      <c r="C59" s="135"/>
+      <c r="D59" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="138"/>
-      <c r="F59" s="137" t="s">
+      <c r="E59" s="135"/>
+      <c r="F59" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G59" s="138"/>
-      <c r="H59" s="139" t="s">
+      <c r="G59" s="135"/>
+      <c r="H59" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I59" s="139"/>
+      <c r="I59" s="136"/>
       <c r="J59" s="121" t="s">
         <v>30</v>
       </c>
@@ -4351,37 +4361,37 @@
       <c r="A60" s="50">
         <v>9</v>
       </c>
-      <c r="B60" s="140" t="s">
+      <c r="B60" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="141"/>
-      <c r="D60" s="146" t="s">
+      <c r="C60" s="147"/>
+      <c r="D60" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="E60" s="147"/>
-      <c r="F60" s="146" t="s">
+      <c r="E60" s="153"/>
+      <c r="F60" s="152" t="s">
         <v>99</v>
       </c>
-      <c r="G60" s="147"/>
-      <c r="H60" s="152" t="s">
+      <c r="G60" s="153"/>
+      <c r="H60" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="I60" s="153"/>
+      <c r="I60" s="168"/>
       <c r="J60" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="K60" s="134"/>
+      <c r="K60" s="173"/>
     </row>
     <row r="61" spans="1:11" ht="10.5" customHeight="1">
       <c r="A61" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="142"/>
-      <c r="C61" s="143"/>
-      <c r="D61" s="148"/>
-      <c r="E61" s="149"/>
-      <c r="F61" s="148"/>
-      <c r="G61" s="149"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="149"/>
+      <c r="D61" s="154"/>
+      <c r="E61" s="155"/>
+      <c r="F61" s="154"/>
+      <c r="G61" s="155"/>
       <c r="H61" s="121" t="s">
         <v>34</v>
       </c>
@@ -4391,18 +4401,18 @@
       <c r="J61" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K61" s="135"/>
+      <c r="K61" s="174"/>
     </row>
     <row r="62" spans="1:11" ht="10.5" customHeight="1">
       <c r="A62" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="142"/>
-      <c r="C62" s="143"/>
-      <c r="D62" s="148"/>
-      <c r="E62" s="149"/>
-      <c r="F62" s="148"/>
-      <c r="G62" s="149"/>
+      <c r="B62" s="148"/>
+      <c r="C62" s="149"/>
+      <c r="D62" s="154"/>
+      <c r="E62" s="155"/>
+      <c r="F62" s="154"/>
+      <c r="G62" s="155"/>
       <c r="H62" s="52" t="s">
         <v>70</v>
       </c>
@@ -4412,18 +4422,18 @@
       <c r="J62" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="K62" s="135"/>
+      <c r="K62" s="174"/>
     </row>
     <row r="63" spans="1:11" ht="10.5" customHeight="1">
       <c r="A63" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B63" s="142"/>
-      <c r="C63" s="143"/>
-      <c r="D63" s="148"/>
-      <c r="E63" s="149"/>
-      <c r="F63" s="148"/>
-      <c r="G63" s="149"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="149"/>
+      <c r="D63" s="154"/>
+      <c r="E63" s="155"/>
+      <c r="F63" s="154"/>
+      <c r="G63" s="155"/>
       <c r="H63" s="121" t="s">
         <v>37</v>
       </c>
@@ -4431,18 +4441,18 @@
         <v>33</v>
       </c>
       <c r="J63" s="121"/>
-      <c r="K63" s="135"/>
+      <c r="K63" s="174"/>
     </row>
     <row r="64" spans="1:11" ht="10.5" customHeight="1">
       <c r="A64" s="53">
         <v>900</v>
       </c>
-      <c r="B64" s="144"/>
-      <c r="C64" s="145"/>
-      <c r="D64" s="150"/>
-      <c r="E64" s="151"/>
-      <c r="F64" s="150"/>
-      <c r="G64" s="151"/>
+      <c r="B64" s="150"/>
+      <c r="C64" s="151"/>
+      <c r="D64" s="156"/>
+      <c r="E64" s="157"/>
+      <c r="F64" s="156"/>
+      <c r="G64" s="157"/>
       <c r="H64" s="52" t="s">
         <v>73</v>
       </c>
@@ -4450,28 +4460,28 @@
         <v>74</v>
       </c>
       <c r="J64" s="50"/>
-      <c r="K64" s="136"/>
+      <c r="K64" s="175"/>
     </row>
     <row r="65" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A65" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="137" t="s">
+      <c r="B65" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="138"/>
-      <c r="D65" s="137" t="s">
+      <c r="C65" s="135"/>
+      <c r="D65" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="E65" s="138"/>
-      <c r="F65" s="137" t="s">
+      <c r="E65" s="135"/>
+      <c r="F65" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="G65" s="138"/>
-      <c r="H65" s="139" t="s">
+      <c r="G65" s="135"/>
+      <c r="H65" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="I65" s="139"/>
+      <c r="I65" s="136"/>
       <c r="J65" s="121" t="s">
         <v>30</v>
       </c>
@@ -4483,35 +4493,35 @@
       <c r="A66" s="50">
         <v>10</v>
       </c>
-      <c r="B66" s="140" t="s">
+      <c r="B66" s="146" t="s">
         <v>110</v>
       </c>
-      <c r="C66" s="141"/>
-      <c r="D66" s="146" t="s">
+      <c r="C66" s="147"/>
+      <c r="D66" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="E66" s="147"/>
-      <c r="F66" s="146" t="s">
+      <c r="E66" s="153"/>
+      <c r="F66" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="G66" s="147"/>
-      <c r="H66" s="152" t="s">
+      <c r="G66" s="153"/>
+      <c r="H66" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="I66" s="153"/>
+      <c r="I66" s="168"/>
       <c r="J66" s="54"/>
-      <c r="K66" s="134"/>
+      <c r="K66" s="173"/>
     </row>
     <row r="67" spans="1:11" ht="10.5" customHeight="1">
       <c r="A67" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="142"/>
-      <c r="C67" s="143"/>
-      <c r="D67" s="148"/>
-      <c r="E67" s="149"/>
-      <c r="F67" s="148"/>
-      <c r="G67" s="149"/>
+      <c r="B67" s="148"/>
+      <c r="C67" s="149"/>
+      <c r="D67" s="154"/>
+      <c r="E67" s="155"/>
+      <c r="F67" s="154"/>
+      <c r="G67" s="155"/>
       <c r="H67" s="121" t="s">
         <v>34</v>
       </c>
@@ -4521,35 +4531,35 @@
       <c r="J67" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K67" s="135"/>
+      <c r="K67" s="174"/>
     </row>
     <row r="68" spans="1:11" ht="10.5" customHeight="1">
       <c r="A68" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B68" s="142"/>
-      <c r="C68" s="143"/>
-      <c r="D68" s="148"/>
-      <c r="E68" s="149"/>
-      <c r="F68" s="148"/>
-      <c r="G68" s="149"/>
+      <c r="B68" s="148"/>
+      <c r="C68" s="149"/>
+      <c r="D68" s="154"/>
+      <c r="E68" s="155"/>
+      <c r="F68" s="154"/>
+      <c r="G68" s="155"/>
       <c r="H68" s="52" t="s">
         <v>71</v>
       </c>
       <c r="I68" s="52"/>
       <c r="J68" s="50"/>
-      <c r="K68" s="135"/>
+      <c r="K68" s="174"/>
     </row>
     <row r="69" spans="1:11" ht="10.5" customHeight="1">
       <c r="A69" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="142"/>
-      <c r="C69" s="143"/>
-      <c r="D69" s="148"/>
-      <c r="E69" s="149"/>
-      <c r="F69" s="148"/>
-      <c r="G69" s="149"/>
+      <c r="B69" s="148"/>
+      <c r="C69" s="149"/>
+      <c r="D69" s="154"/>
+      <c r="E69" s="155"/>
+      <c r="F69" s="154"/>
+      <c r="G69" s="155"/>
       <c r="H69" s="121" t="s">
         <v>37</v>
       </c>
@@ -4557,24 +4567,24 @@
         <v>33</v>
       </c>
       <c r="J69" s="121"/>
-      <c r="K69" s="135"/>
+      <c r="K69" s="174"/>
     </row>
     <row r="70" spans="1:11" ht="10.5" customHeight="1">
       <c r="A70" s="53">
         <v>845</v>
       </c>
-      <c r="B70" s="144"/>
-      <c r="C70" s="145"/>
-      <c r="D70" s="150"/>
-      <c r="E70" s="151"/>
-      <c r="F70" s="150"/>
-      <c r="G70" s="151"/>
+      <c r="B70" s="150"/>
+      <c r="C70" s="151"/>
+      <c r="D70" s="156"/>
+      <c r="E70" s="157"/>
+      <c r="F70" s="156"/>
+      <c r="G70" s="157"/>
       <c r="H70" s="52" t="s">
         <v>73</v>
       </c>
       <c r="I70" s="52"/>
       <c r="J70" s="50"/>
-      <c r="K70" s="136"/>
+      <c r="K70" s="175"/>
     </row>
     <row r="71" spans="1:11" s="131" customFormat="1" ht="10.5" customHeight="1"/>
     <row r="72" spans="1:11" s="131" customFormat="1" ht="10.5" customHeight="1"/>
@@ -4934,6 +4944,83 @@
     </row>
   </sheetData>
   <mergeCells count="93">
+    <mergeCell ref="K66:K70"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="B66:C70"/>
+    <mergeCell ref="D66:E70"/>
+    <mergeCell ref="F66:G70"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B60:C64"/>
+    <mergeCell ref="D60:E64"/>
+    <mergeCell ref="F60:G64"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="K60:K64"/>
+    <mergeCell ref="K48:K52"/>
+    <mergeCell ref="K54:K58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:E58"/>
+    <mergeCell ref="F54:G58"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="B48:C52"/>
+    <mergeCell ref="D48:E52"/>
+    <mergeCell ref="F48:G52"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B42:C46"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="D42:E46"/>
+    <mergeCell ref="F42:G46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="K42:K46"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="F9:G13"/>
+    <mergeCell ref="F21:G25"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="F15:G19"/>
+    <mergeCell ref="K15:K19"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="B8:C8"/>
@@ -4950,83 +5037,6 @@
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="F9:G13"/>
-    <mergeCell ref="F21:G25"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="F15:G19"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B42:C46"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="D42:E46"/>
-    <mergeCell ref="F42:G46"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B48:C52"/>
-    <mergeCell ref="D48:E52"/>
-    <mergeCell ref="F48:G52"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="K48:K52"/>
-    <mergeCell ref="K54:K58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B54:C58"/>
-    <mergeCell ref="D54:E58"/>
-    <mergeCell ref="F54:G58"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B60:C64"/>
-    <mergeCell ref="D60:E64"/>
-    <mergeCell ref="F60:G64"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K60:K64"/>
-    <mergeCell ref="K66:K70"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="B66:C70"/>
-    <mergeCell ref="D66:E70"/>
-    <mergeCell ref="F66:G70"/>
-    <mergeCell ref="H66:I66"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H42:I42">

</xml_diff>